<commit_message>
Update : Columname Add : FindRecipe.csv
</commit_message>
<xml_diff>
--- a/Assets/Resources/Recipe.xlsx
+++ b/Assets/Resources/Recipe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SM-PC\Documents\GitHub\Tycoon\Assets\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SM-PC\Documents\Tycoon\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9226FA4C-736B-4B30-9C63-C95D02817ADE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26269490-B184-4207-9466-175276E0CDE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8976" xr2:uid="{B64F3FDA-0D76-4033-A8A5-2E0E2E6B863B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8976" xr2:uid="{DA8289E2-CD5B-4A34-BB33-B35A7C1DE5AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="94">
   <si>
     <t>요리_ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,26 +64,28 @@
     <t>재료3_ID</t>
   </si>
   <si>
-    <t>과정1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>과정2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>과정3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>컷씬1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>컷씬2</t>
-  </si>
-  <si>
-    <t>컷씬3</t>
+    <t>과정1_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과정2_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과정3_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컷씬1_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컷씬2_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컷씬3_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>recipe0001</t>
@@ -102,8 +104,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>찌기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>steam</t>
   </si>
   <si>
     <t>recipe0002</t>
@@ -117,8 +118,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>튀기기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>fry</t>
   </si>
   <si>
     <t>recipe0003</t>
@@ -132,8 +132,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>끓이기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>boil</t>
   </si>
   <si>
     <t>recipe0004</t>
@@ -151,8 +150,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>굽기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>roast</t>
   </si>
   <si>
     <t>recipe0005</t>
@@ -177,8 +175,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>볶기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>stirfry</t>
   </si>
   <si>
     <t>recipe0007</t>
@@ -237,8 +234,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>졸이기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>boildown</t>
   </si>
   <si>
     <t>recipe0011</t>
@@ -376,6 +372,10 @@
   </si>
   <si>
     <t>감자 없는 감자탕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -491,249 +491,257 @@
       <sheetData sheetId="8">
         <row r="2">
           <cell r="A2" t="str">
-            <v>건식 전투식량 블럭</v>
+            <v>x</v>
           </cell>
           <cell r="B2" t="str">
-            <v>food0001</v>
+            <v>null</v>
           </cell>
         </row>
         <row r="3">
           <cell r="A3" t="str">
-            <v>노래하는 옥수수</v>
+            <v>건식 전투식량 블럭</v>
           </cell>
           <cell r="B3" t="str">
-            <v>food0002</v>
+            <v>food0001</v>
           </cell>
         </row>
         <row r="4">
           <cell r="A4" t="str">
-            <v>굽은 뿔 산양 위장 주머니</v>
+            <v>노래하는 옥수수</v>
           </cell>
           <cell r="B4" t="str">
-            <v>food0003</v>
+            <v>food0002</v>
           </cell>
         </row>
         <row r="5">
           <cell r="A5" t="str">
-            <v>별바라기</v>
+            <v>굽은 뿔 산양 위장 주머니</v>
           </cell>
           <cell r="B5" t="str">
-            <v>food0004</v>
+            <v>food0003</v>
           </cell>
         </row>
         <row r="6">
           <cell r="A6" t="str">
-            <v>밀가루 반죽</v>
+            <v>별바라기</v>
           </cell>
           <cell r="B6" t="str">
-            <v>food0005</v>
+            <v>food0004</v>
           </cell>
         </row>
         <row r="7">
           <cell r="A7" t="str">
-            <v>비스킷 반죽</v>
+            <v>밀가루 반죽</v>
           </cell>
           <cell r="B7" t="str">
-            <v>food0006</v>
+            <v>food0005</v>
           </cell>
         </row>
         <row r="8">
           <cell r="A8" t="str">
-            <v>망치새 알</v>
+            <v>비스킷 반죽</v>
           </cell>
           <cell r="B8" t="str">
-            <v>food0007</v>
+            <v>food0006</v>
           </cell>
         </row>
         <row r="9">
           <cell r="A9" t="str">
-            <v>오브리제 XII 시약</v>
+            <v>망치새 알</v>
           </cell>
           <cell r="B9" t="str">
-            <v>food0008</v>
+            <v>food0007</v>
           </cell>
         </row>
         <row r="10">
           <cell r="A10" t="str">
-            <v>마늘</v>
+            <v>오브리제 XII 시약</v>
           </cell>
           <cell r="B10" t="str">
-            <v>food0009</v>
+            <v>food0008</v>
           </cell>
         </row>
         <row r="11">
           <cell r="A11" t="str">
-            <v>화살촉 새우</v>
+            <v>마늘</v>
           </cell>
           <cell r="B11" t="str">
-            <v>food0010</v>
+            <v>food0009</v>
           </cell>
         </row>
         <row r="12">
           <cell r="A12" t="str">
-            <v>도둑문어</v>
+            <v>화살촉 새우</v>
           </cell>
           <cell r="B12" t="str">
-            <v>food0011</v>
+            <v>food0010</v>
           </cell>
         </row>
         <row r="13">
           <cell r="A13" t="str">
-            <v>당근</v>
+            <v>도둑문어</v>
           </cell>
           <cell r="B13" t="str">
-            <v>food0012</v>
+            <v>food0011</v>
           </cell>
         </row>
         <row r="14">
           <cell r="A14" t="str">
-            <v>와이번 뼈</v>
+            <v>당근</v>
           </cell>
           <cell r="B14" t="str">
-            <v>food0013</v>
+            <v>food0012</v>
           </cell>
         </row>
         <row r="15">
           <cell r="A15" t="str">
-            <v>면 반죽</v>
+            <v>와이번 뼈</v>
           </cell>
           <cell r="B15" t="str">
-            <v>food0014</v>
+            <v>food0013</v>
           </cell>
         </row>
         <row r="16">
           <cell r="A16" t="str">
-            <v>토마토</v>
+            <v>면 반죽</v>
           </cell>
           <cell r="B16" t="str">
-            <v>food0015</v>
+            <v>food0014</v>
           </cell>
         </row>
         <row r="17">
           <cell r="A17" t="str">
-            <v>코카트리스 알</v>
+            <v>토마토</v>
           </cell>
           <cell r="B17" t="str">
-            <v>food0016</v>
+            <v>food0015</v>
           </cell>
         </row>
         <row r="18">
           <cell r="A18" t="str">
-            <v>걸어다니는버섯</v>
+            <v>코카트리스 알</v>
           </cell>
           <cell r="B18" t="str">
-            <v>food0017</v>
+            <v>food0016</v>
           </cell>
         </row>
         <row r="19">
           <cell r="A19" t="str">
-            <v>바실리크 다리살</v>
+            <v>걸어다니는버섯</v>
           </cell>
           <cell r="B19" t="str">
-            <v>food0018</v>
+            <v>food0017</v>
           </cell>
         </row>
         <row r="20">
           <cell r="A20" t="str">
-            <v>양파</v>
+            <v>바실리크 다리살</v>
           </cell>
           <cell r="B20" t="str">
-            <v>food0019</v>
+            <v>food0018</v>
           </cell>
         </row>
         <row r="21">
           <cell r="A21" t="str">
-            <v>곰 고기</v>
+            <v>양파</v>
           </cell>
           <cell r="B21" t="str">
-            <v>food0020</v>
+            <v>food0019</v>
           </cell>
         </row>
         <row r="22">
           <cell r="A22" t="str">
-            <v>람다 샤우팅 레드와인</v>
+            <v>곰 고기</v>
           </cell>
           <cell r="B22" t="str">
-            <v>food0021</v>
+            <v>food0020</v>
           </cell>
         </row>
         <row r="23">
           <cell r="A23" t="str">
-            <v>쌀</v>
+            <v>람다 샤우팅 레드와인</v>
           </cell>
           <cell r="B23" t="str">
-            <v>food0022</v>
+            <v>food0021</v>
           </cell>
         </row>
         <row r="24">
           <cell r="A24" t="str">
-            <v>설산 이끼</v>
+            <v>쌀</v>
           </cell>
           <cell r="B24" t="str">
-            <v>food0023</v>
+            <v>food0022</v>
           </cell>
         </row>
         <row r="25">
           <cell r="A25" t="str">
-            <v>큰 어금니 멧돼지 고기</v>
+            <v>설산 이끼</v>
           </cell>
           <cell r="B25" t="str">
-            <v>food0024</v>
+            <v>food0023</v>
           </cell>
         </row>
         <row r="26">
           <cell r="A26" t="str">
-            <v>코카트리스 발</v>
+            <v>큰 어금니 멧돼지 고기</v>
           </cell>
           <cell r="B26" t="str">
-            <v>food0025</v>
+            <v>food0024</v>
           </cell>
         </row>
         <row r="27">
           <cell r="A27" t="str">
-            <v>설산 와이번 고기</v>
+            <v>코카트리스 발</v>
           </cell>
           <cell r="B27" t="str">
-            <v>food0026</v>
+            <v>food0025</v>
           </cell>
         </row>
         <row r="28">
           <cell r="A28" t="str">
-            <v>람다 카레 블록</v>
+            <v>설산 와이번 고기</v>
           </cell>
           <cell r="B28" t="str">
-            <v>food0027</v>
+            <v>food0026</v>
           </cell>
         </row>
         <row r="29">
           <cell r="A29" t="str">
-            <v>감자</v>
+            <v>람다 카레 블록</v>
           </cell>
           <cell r="B29" t="str">
-            <v>food0028</v>
+            <v>food0027</v>
           </cell>
         </row>
         <row r="30">
           <cell r="A30" t="str">
-            <v>구멍풀 뿌리</v>
+            <v>감자</v>
           </cell>
           <cell r="B30" t="str">
-            <v>food0029</v>
+            <v>food0028</v>
           </cell>
         </row>
         <row r="31">
           <cell r="A31" t="str">
-            <v>와이번 알</v>
+            <v>구멍풀 뿌리</v>
           </cell>
           <cell r="B31" t="str">
-            <v>food0030</v>
+            <v>food0029</v>
           </cell>
         </row>
         <row r="32">
           <cell r="A32" t="str">
+            <v>와이번 알</v>
+          </cell>
+          <cell r="B32" t="str">
+            <v>food0030</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33" t="str">
             <v>저무는 달의 잎사귀</v>
           </cell>
-          <cell r="B32" t="str">
+          <cell r="B33" t="str">
             <v>food0031</v>
           </cell>
         </row>
@@ -1040,11 +1048,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36626870-4974-45C2-A8F6-4476B6737EFA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DE86B3-9EE4-45BC-903D-C894E702AFC9}">
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O21"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1119,13 +1127,13 @@
         <f>VLOOKUP(D2,[1]요리재료!$A$2:$B$98,2,0)</f>
         <v>food0001</v>
       </c>
-      <c r="H2" t="e">
+      <c r="H2" t="str">
         <f>VLOOKUP(E2,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I2" t="e">
+        <v>null</v>
+      </c>
+      <c r="I2" t="str">
         <f>VLOOKUP(F2,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
+        <v>null</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>
@@ -1166,13 +1174,13 @@
         <f>VLOOKUP(D3,[1]요리재료!$A$2:$B$98,2,0)</f>
         <v>food0002</v>
       </c>
-      <c r="H3" t="e">
+      <c r="H3" t="str">
         <f>VLOOKUP(E3,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I3" t="e">
+        <v>null</v>
+      </c>
+      <c r="I3" t="str">
         <f>VLOOKUP(F3,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
+        <v>null</v>
       </c>
       <c r="J3" t="s">
         <v>23</v>
@@ -1213,13 +1221,13 @@
         <f>VLOOKUP(D4,[1]요리재료!$A$2:$B$98,2,0)</f>
         <v>food0003</v>
       </c>
-      <c r="H4" t="e">
+      <c r="H4" t="str">
         <f>VLOOKUP(E4,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I4" t="e">
+        <v>null</v>
+      </c>
+      <c r="I4" t="str">
         <f>VLOOKUP(F4,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
+        <v>null</v>
       </c>
       <c r="J4" t="s">
         <v>27</v>
@@ -1264,9 +1272,9 @@
         <f>VLOOKUP(E5,[1]요리재료!$A$2:$B$98,2,0)</f>
         <v>food0005</v>
       </c>
-      <c r="I5" t="e">
+      <c r="I5" t="str">
         <f>VLOOKUP(F5,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
+        <v>null</v>
       </c>
       <c r="J5" t="s">
         <v>32</v>
@@ -1304,13 +1312,13 @@
         <f>VLOOKUP(D6,[1]요리재료!$A$2:$B$98,2,0)</f>
         <v>food0006</v>
       </c>
-      <c r="H6" t="e">
+      <c r="H6" t="str">
         <f>VLOOKUP(E6,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I6" t="e">
+        <v>null</v>
+      </c>
+      <c r="I6" t="str">
         <f>VLOOKUP(F6,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
+        <v>null</v>
       </c>
       <c r="J6" t="s">
         <v>32</v>
@@ -1351,13 +1359,13 @@
         <f>VLOOKUP(D7,[1]요리재료!$A$2:$B$98,2,0)</f>
         <v>food0007</v>
       </c>
-      <c r="H7" t="e">
+      <c r="H7" t="str">
         <f>VLOOKUP(E7,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I7" t="e">
+        <v>null</v>
+      </c>
+      <c r="I7" t="str">
         <f>VLOOKUP(F7,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
+        <v>null</v>
       </c>
       <c r="J7" t="s">
         <v>39</v>
@@ -1398,13 +1406,13 @@
         <f>VLOOKUP(D8,[1]요리재료!$A$2:$B$98,2,0)</f>
         <v>food0008</v>
       </c>
-      <c r="H8" t="e">
+      <c r="H8" t="str">
         <f>VLOOKUP(E8,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I8" t="e">
+        <v>null</v>
+      </c>
+      <c r="I8" t="str">
         <f>VLOOKUP(F8,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
+        <v>null</v>
       </c>
       <c r="J8" t="s">
         <v>27</v>
@@ -1445,13 +1453,12 @@
         <f>VLOOKUP(D9,[1]요리재료!$A$2:$B$98,2,0)</f>
         <v>food0009</v>
       </c>
-      <c r="H9" t="e">
-        <f>VLOOKUP(E9,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I9" t="e">
+      <c r="H9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" t="str">
         <f>VLOOKUP(F9,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
+        <v>null</v>
       </c>
       <c r="J9" t="s">
         <v>23</v>
@@ -1493,9 +1500,9 @@
         <f>VLOOKUP(E10,[1]요리재료!$A$2:$B$98,2,0)</f>
         <v>food0005</v>
       </c>
-      <c r="I10" t="e">
+      <c r="I10" t="str">
         <f>VLOOKUP(F10,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
+        <v>null</v>
       </c>
       <c r="J10" t="s">
         <v>27</v>
@@ -1578,9 +1585,9 @@
         <f>VLOOKUP(E12,[1]요리재료!$A$2:$B$98,2,0)</f>
         <v>food0016</v>
       </c>
-      <c r="I12" t="e">
+      <c r="I12" t="str">
         <f>VLOOKUP(F12,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
+        <v>null</v>
       </c>
       <c r="J12" t="s">
         <v>39</v>
@@ -1826,13 +1833,13 @@
         <f>VLOOKUP(D18,[1]요리재료!$A$2:$B$98,2,0)</f>
         <v>food0025</v>
       </c>
-      <c r="H18" t="e">
+      <c r="H18" t="str">
         <f>VLOOKUP(E18,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I18" t="e">
+        <v>null</v>
+      </c>
+      <c r="I18" t="str">
         <f>VLOOKUP(F18,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
+        <v>null</v>
       </c>
       <c r="J18" t="s">
         <v>39</v>
@@ -1959,9 +1966,9 @@
         <f>VLOOKUP(E21,[1]요리재료!$A$2:$B$98,2,0)</f>
         <v>food0023</v>
       </c>
-      <c r="I21" t="e">
+      <c r="I21" t="str">
         <f>VLOOKUP(F21,[1]요리재료!$A$2:$B$98,2,0)</f>
-        <v>#N/A</v>
+        <v>null</v>
       </c>
       <c r="J21" t="s">
         <v>27</v>

</xml_diff>